<commit_message>
updated the Test Case v1.0.xlsx
</commit_message>
<xml_diff>
--- a/INITIAL DOCS (.docx)/Test Case v1.0.xlsx
+++ b/INITIAL DOCS (.docx)/Test Case v1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asiapacificcollege.sharepoint.com/sites/QUALITYMI201MI203T12023-2024/Shared Documents/Group 04 - Team AV/Documents/INITIAL DOCS (.docx)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jetas\OneDrive - Asia Pacific College\Desktop\APC_2023_2024_T1_G04_Team_AV\INITIAL DOCS (.docx)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="354" documentId="11_B63FE2A2ED2272DCC0CB705FC6BDCDCABA86F51E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCF87F8C-5673-4A85-A8C9-069E8D33AE5E}"/>
+  <xr:revisionPtr revIDLastSave="355" documentId="11_B63FE2A2ED2272DCC0CB705FC6BDCDCABA86F51E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EB4C7C8-6A17-4CD1-918C-6AC9650F3144}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Authentication" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="133">
   <si>
     <t>TEST DESCRIPTION</t>
   </si>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t>BSSVTC01 - BSSVTC24</t>
+  </si>
+  <si>
+    <t>Sofia Villamin</t>
   </si>
 </sst>
 </file>
@@ -886,34 +889,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="363">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="147">
     <dxf>
       <font>
         <color theme="1"/>
@@ -989,6 +965,60 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
@@ -1016,6 +1046,23 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1047,18 +1094,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1095,6 +1135,23 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1120,33 +1177,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
@@ -1174,6 +1204,23 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1226,6 +1273,33 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
@@ -1253,6 +1327,23 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1284,18 +1375,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1332,6 +1416,23 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1411,6 +1512,23 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1436,33 +1554,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
@@ -1521,11 +1612,18 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1583,40 +1681,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1675,23 +1739,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1723,11 +1770,18 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1764,23 +1818,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1802,11 +1839,28 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2032,18 +2086,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2096,2164 +2143,6 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4754,7 +2643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34081978-D0BE-495A-A8D6-1A011FC4BDD5}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -5657,351 +3546,351 @@
     <mergeCell ref="A28:L28"/>
   </mergeCells>
   <conditionalFormatting sqref="B2 I14:L20">
-    <cfRule type="containsText" dxfId="175" priority="170" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="146" priority="170" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="171" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="145" priority="171" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12 I14:I20 I24:I27 I29">
-    <cfRule type="containsText" dxfId="173" priority="158" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="144" priority="158" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="159" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="143" priority="159" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12 K9:K12 K35 I24:I27 K24:K27">
-    <cfRule type="containsText" dxfId="171" priority="166" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="142" priority="166" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="167" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="141" priority="167" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="168" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="140" priority="168" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:L20">
-    <cfRule type="containsText" dxfId="168" priority="163" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="139" priority="163" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="167" priority="169" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="138" priority="169" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:L19">
-    <cfRule type="containsText" dxfId="166" priority="151" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="137" priority="151" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="152" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="136" priority="152" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="containsText" dxfId="164" priority="148" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="135" priority="148" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="149" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="134" priority="149" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:L19">
-    <cfRule type="containsText" dxfId="162" priority="150" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="133" priority="150" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:L18">
-    <cfRule type="containsText" dxfId="161" priority="141" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="132" priority="141" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="142" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="131" priority="142" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="159" priority="138" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="130" priority="138" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="139" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="129" priority="139" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:L18">
-    <cfRule type="containsText" dxfId="157" priority="140" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="128" priority="140" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:L21">
-    <cfRule type="containsText" dxfId="153" priority="118" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="127" priority="118" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",J21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="119" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="126" priority="119" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:L21">
-    <cfRule type="containsText" dxfId="151" priority="117" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="125" priority="117" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:L22">
-    <cfRule type="containsText" dxfId="150" priority="108" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="124" priority="108" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",J22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="109" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="123" priority="109" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",J22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:L22">
-    <cfRule type="containsText" dxfId="148" priority="107" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="122" priority="107" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",J22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="147" priority="102" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="121" priority="102" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="103" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="120" priority="103" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="104" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="119" priority="104" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="144" priority="99" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="118" priority="99" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="100" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="117" priority="100" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="101" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="116" priority="101" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="141" priority="89" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="115" priority="89" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="90" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="114" priority="90" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="139" priority="86" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="113" priority="86" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="87" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="112" priority="87" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="88" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="111" priority="88" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="136" priority="83" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="110" priority="83" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="84" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="109" priority="84" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="85" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="108" priority="85" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="133" priority="73" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="107" priority="73" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="74" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="106" priority="74" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="131" priority="70" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="105" priority="70" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="71" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="104" priority="71" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="72" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="103" priority="72" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="128" priority="67" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="102" priority="67" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="68" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="101" priority="68" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="69" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="100" priority="69" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="125" priority="57" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="99" priority="57" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="58" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="98" priority="58" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="123" priority="54" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="97" priority="54" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="55" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="96" priority="55" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="56" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="95" priority="56" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="120" priority="51" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="94" priority="51" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="52" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="93" priority="52" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="53" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="92" priority="53" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="117" priority="41" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="91" priority="41" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="42" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="90" priority="42" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="115" priority="38" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="89" priority="38" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="39" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="88" priority="39" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="40" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="87" priority="40" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="112" priority="35" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="86" priority="35" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="36" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="85" priority="36" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="37" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="84" priority="37" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="109" priority="33" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="83" priority="33" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="34" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="82" priority="34" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="107" priority="30" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="81" priority="30" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="31" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="80" priority="31" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="32" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="79" priority="32" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="104" priority="27" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="78" priority="27" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="28" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="77" priority="28" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="29" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="76" priority="29" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="101" priority="17" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="75" priority="17" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="18" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="74" priority="18" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="99" priority="14" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="73" priority="14" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="15" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="72" priority="15" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="16" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="71" priority="16" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="96" priority="11" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="70" priority="11" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="12" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="69" priority="12" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="13" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="68" priority="13" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="67" priority="9" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="66" priority="10" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="65" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="64" priority="7" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="63" priority="8" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="60" priority="1" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="59" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="58" priority="3" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6022,8 +3911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0768D9F1-4234-49C1-8BF8-F5440FF0513C}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6106,7 +3995,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>45</v>
+        <v>132</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>19</v>
@@ -6587,119 +4476,119 @@
     <mergeCell ref="A15:L15"/>
   </mergeCells>
   <conditionalFormatting sqref="B2 I16:L22">
-    <cfRule type="containsText" dxfId="362" priority="56" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="57" priority="56" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="361" priority="57" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12 I16:I22">
-    <cfRule type="containsText" dxfId="360" priority="49" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="359" priority="50" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="54" priority="50" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12 K9:K12">
-    <cfRule type="containsText" dxfId="358" priority="52" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="53" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="356" priority="54" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:L22">
-    <cfRule type="containsText" dxfId="355" priority="51" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="354" priority="55" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="49" priority="55" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:L21">
-    <cfRule type="containsText" dxfId="353" priority="47" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="352" priority="48" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="351" priority="44" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="350" priority="45" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:L21">
-    <cfRule type="containsText" dxfId="349" priority="46" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:L20">
-    <cfRule type="containsText" dxfId="348" priority="42" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="347" priority="43" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="346" priority="39" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="40" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="40" priority="40" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:L20">
-    <cfRule type="containsText" dxfId="344" priority="41" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="343" priority="11" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="38" priority="11" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="342" priority="12" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="37" priority="12" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13 K13">
-    <cfRule type="containsText" dxfId="341" priority="13" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="36" priority="13" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="340" priority="14" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="339" priority="15" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="338" priority="1" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="337" priority="2" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14 K14">
-    <cfRule type="containsText" dxfId="336" priority="3" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="335" priority="4" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="30" priority="4" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="334" priority="5" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6720,7 +4609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1936D42-EC5B-4A23-B077-0845695AD7C1}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -7273,119 +5162,119 @@
     <mergeCell ref="A15:L15"/>
   </mergeCells>
   <conditionalFormatting sqref="B2 I16:L22">
-    <cfRule type="containsText" dxfId="333" priority="28" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="332" priority="29" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12 I16:I22">
-    <cfRule type="containsText" dxfId="331" priority="21" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="330" priority="22" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12 K9:K12">
-    <cfRule type="containsText" dxfId="329" priority="24" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="328" priority="25" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="327" priority="26" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:L22">
-    <cfRule type="containsText" dxfId="326" priority="23" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="325" priority="27" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:L21">
-    <cfRule type="containsText" dxfId="324" priority="19" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="323" priority="20" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="322" priority="16" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="321" priority="17" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:L21">
-    <cfRule type="containsText" dxfId="320" priority="18" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:L20">
-    <cfRule type="containsText" dxfId="319" priority="14" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="318" priority="15" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="317" priority="11" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="316" priority="12" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:L20">
-    <cfRule type="containsText" dxfId="315" priority="13" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="314" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="313" priority="7" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13 K13">
-    <cfRule type="containsText" dxfId="312" priority="8" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="311" priority="9" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="310" priority="10" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="309" priority="1" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="308" priority="2" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14 K14">
-    <cfRule type="containsText" dxfId="307" priority="3" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="306" priority="4" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="305" priority="5" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7403,26 +5292,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf23f84-f8bc-4e67-ab33-02601704301c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006E296302A21A604AB30B08CDD982AED5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a2e24ddf9d3ff53ecfb88a36bb32033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8bf23f84-f8bc-4e67-ab33-02601704301c" xmlns:ns3="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85173b95bb32453a086c351bdaabae72" ns2:_="" ns3:_="">
     <xsd:import namespace="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
@@ -7645,32 +5514,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C8A6C0-18BD-4AC2-9685-64609DD34696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf23f84-f8bc-4e67-ab33-02601704301c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F65EC3E-6CD5-4311-8679-E96C36401EA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="becc6418-98a4-4be0-bb44-3ce60d9e2ca3"/>
-    <ds:schemaRef ds:uri="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDBCEFB4-C136-4DFA-9FAE-3B56459231A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7687,4 +5551,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F65EC3E-6CD5-4311-8679-E96C36401EA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="becc6418-98a4-4be0-bb44-3ce60d9e2ca3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C8A6C0-18BD-4AC2-9685-64609DD34696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update INITIAL DOCS (.docx)/Test Case v1.0.xlsx
</commit_message>
<xml_diff>
--- a/INITIAL DOCS (.docx)/Test Case v1.0.xlsx
+++ b/INITIAL DOCS (.docx)/Test Case v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jetas\OneDrive - Asia Pacific College\Desktop\APC_2023_2024_T1_G04_Team_AV\INITIAL DOCS (.docx)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofIa\Desktop\APC_2023_2024_T1_G04_Team_AV\INITIAL DOCS (.docx)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="355" documentId="11_B63FE2A2ED2272DCC0CB705FC6BDCDCABA86F51E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EB4C7C8-6A17-4CD1-918C-6AC9650F3144}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBAD207-1346-4D30-9A94-C4B02FCBB0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Authentication" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="134">
   <si>
     <t>TEST DESCRIPTION</t>
   </si>
@@ -133,15 +133,6 @@
   </si>
   <si>
     <t>System will notify that customer has successfully created an account</t>
-  </si>
-  <si>
-    <t>TC10</t>
-  </si>
-  <si>
-    <t>TC11</t>
-  </si>
-  <si>
-    <t>TC12</t>
   </si>
   <si>
     <t>System will notify that email is invalid.</t>
@@ -449,6 +440,18 @@
   </si>
   <si>
     <t>Sofia Villamin</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>TC04</t>
   </si>
 </sst>
 </file>
@@ -889,7 +892,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="147">
+  <dxfs count="87">
     <dxf>
       <font>
         <color theme="1"/>
@@ -923,6 +926,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -971,45 +1018,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1040,33 +1053,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
@@ -1104,6 +1090,57 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1135,18 +1172,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1204,23 +1234,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1252,23 +1265,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1279,18 +1275,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1306,6 +1295,23 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -1327,18 +1333,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1355,31 +1354,18 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1400,17 +1386,24 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1421,13 +1414,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1533,18 +1519,45 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1565,6 +1578,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1576,6 +1599,16 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1591,39 +1624,53 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1644,17 +1691,37 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1666,668 +1733,6 @@
         <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2647,22 +2052,22 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="11" width="21.140625" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="11" width="21.109375" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2682,7 +2087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -2690,10 +2095,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -2702,7 +2107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2719,15 +2124,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>19</v>
@@ -2736,7 +2141,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -2746,7 +2151,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -2756,7 +2161,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
@@ -2785,7 +2190,7 @@
         <v>28</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>30</v>
@@ -2794,9 +2199,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -2810,21 +2215,21 @@
       <c r="K8" s="39"/>
       <c r="L8" s="40"/>
     </row>
-    <row r="9" spans="1:12" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>31</v>
@@ -2840,21 +2245,21 @@
       <c r="K9" s="22"/>
       <c r="L9" s="23"/>
     </row>
-    <row r="10" spans="1:12" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>62</v>
-      </c>
       <c r="D10" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>31</v>
@@ -2870,27 +2275,27 @@
       <c r="K10" s="4"/>
       <c r="L10" s="27"/>
     </row>
-    <row r="11" spans="1:12" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>55</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="4" t="s">
@@ -2900,27 +2305,27 @@
       <c r="K11" s="4"/>
       <c r="L11" s="27"/>
     </row>
-    <row r="12" spans="1:12" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="4" t="s">
@@ -2930,9 +2335,9 @@
       <c r="K12" s="4"/>
       <c r="L12" s="27"/>
     </row>
-    <row r="13" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
@@ -2946,18 +2351,18 @@
       <c r="K13" s="39"/>
       <c r="L13" s="40"/>
     </row>
-    <row r="14" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="26" t="s">
@@ -2974,22 +2379,22 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="273.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="273.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B15" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="24" t="s">
-        <v>63</v>
-      </c>
       <c r="D15" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="26" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G15" s="26" t="s">
         <v>31</v>
@@ -3002,18 +2407,18 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="26" t="s">
@@ -3030,18 +2435,18 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="26" t="s">
@@ -3058,18 +2463,18 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="26" t="s">
@@ -3086,18 +2491,18 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="259.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="259.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="26" t="s">
@@ -3114,22 +2519,22 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="275.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="275.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G20" s="26" t="s">
         <v>31</v>
@@ -3142,22 +2547,22 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="279" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="279" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G21" s="26" t="s">
         <v>31</v>
@@ -3170,18 +2575,18 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="288.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="288.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="26" t="s">
@@ -3198,9 +2603,9 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
@@ -3214,25 +2619,25 @@
       <c r="K23" s="39"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:12" ht="246" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="246" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H24" s="26"/>
       <c r="I24" s="4" t="s">
@@ -3242,25 +2647,25 @@
       <c r="K24" s="4"/>
       <c r="L24" s="27"/>
     </row>
-    <row r="25" spans="1:12" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="4" t="s">
@@ -3270,25 +2675,25 @@
       <c r="K25" s="4"/>
       <c r="L25" s="27"/>
     </row>
-    <row r="26" spans="1:12" ht="269.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="269.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H26" s="21"/>
       <c r="I26" s="22" t="s">
@@ -3298,25 +2703,25 @@
       <c r="K26" s="22"/>
       <c r="L26" s="23"/>
     </row>
-    <row r="27" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G27" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="4" t="s">
@@ -3326,9 +2731,9 @@
       <c r="K27" s="4"/>
       <c r="L27" s="27"/>
     </row>
-    <row r="28" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="38" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
@@ -3342,18 +2747,18 @@
       <c r="K28" s="39"/>
       <c r="L28" s="40"/>
     </row>
-    <row r="29" spans="1:12" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="26" t="s">
@@ -3370,18 +2775,18 @@
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
     </row>
-    <row r="30" spans="1:12" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="26" t="s">
@@ -3398,18 +2803,18 @@
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
     </row>
-    <row r="31" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="26" t="s">
@@ -3426,25 +2831,25 @@
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
     </row>
-    <row r="32" spans="1:12" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H32" s="26"/>
       <c r="I32" s="4" t="s">
@@ -3454,18 +2859,18 @@
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
     </row>
-    <row r="33" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="26" t="s">
@@ -3482,25 +2887,25 @@
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
     </row>
-    <row r="34" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="4" t="s">
@@ -3510,25 +2915,25 @@
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
     </row>
-    <row r="35" spans="1:12" ht="264" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="264" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="4" t="s">
@@ -3546,352 +2951,216 @@
     <mergeCell ref="A28:L28"/>
   </mergeCells>
   <conditionalFormatting sqref="B2 I14:L20">
-    <cfRule type="containsText" dxfId="146" priority="170" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="86" priority="171" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="170" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="171" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="containsText" dxfId="84" priority="169" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12 I14:I20 I24:I27 I29">
-    <cfRule type="containsText" dxfId="144" priority="158" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="83" priority="159" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I12 I24:I27 K9:K12 K24:K27 K35">
+    <cfRule type="containsText" dxfId="82" priority="166" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I12 K9:K12 I24:I27 K24:K27 K35">
+    <cfRule type="containsText" dxfId="81" priority="168" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="167" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I20 I29 I9:I12 I24:I27">
+    <cfRule type="containsText" dxfId="79" priority="158" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="159" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",I9)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I12 K9:K12 K35 I24:I27 K24:K27">
-    <cfRule type="containsText" dxfId="142" priority="166" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="167" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="168" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+  <conditionalFormatting sqref="I18:I19">
+    <cfRule type="containsText" dxfId="78" priority="139" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="138" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21:I22">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",I21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="containsText" dxfId="74" priority="104" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="103" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="102" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29:I30">
+    <cfRule type="containsText" dxfId="71" priority="87" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="86" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="88" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="containsText" dxfId="68" priority="90" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="89" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30:I31">
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="71" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="70" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="containsText" dxfId="63" priority="73" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="74" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31:I32">
+    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="55" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="56" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32:I33">
+    <cfRule type="containsText" dxfId="56" priority="38" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="39" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="40" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="containsText" dxfId="53" priority="42" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="41" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33:I34">
+    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="30" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="32" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="containsText" dxfId="48" priority="33" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="34" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34:I35">
+    <cfRule type="containsText" dxfId="46" priority="16" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="15" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="14" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="containsText" dxfId="43" priority="12" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="18" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="17" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="13" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="11" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:L20">
-    <cfRule type="containsText" dxfId="139" priority="163" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="38" priority="163" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="138" priority="169" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
+  <conditionalFormatting sqref="I18:L19">
+    <cfRule type="containsText" dxfId="37" priority="140" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="141" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="142" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I19:L19">
-    <cfRule type="containsText" dxfId="137" priority="151" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="152" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="containsText" dxfId="135" priority="148" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="149" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19:L19">
-    <cfRule type="containsText" dxfId="133" priority="150" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:L18">
-    <cfRule type="containsText" dxfId="132" priority="141" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="142" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="130" priority="138" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="139" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:L18">
-    <cfRule type="containsText" dxfId="128" priority="140" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21:L21">
-    <cfRule type="containsText" dxfId="127" priority="118" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",J21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="119" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",J21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21:L21">
-    <cfRule type="containsText" dxfId="125" priority="117" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",J21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22:L22">
-    <cfRule type="containsText" dxfId="124" priority="108" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",J22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="109" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",J22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22:L22">
-    <cfRule type="containsText" dxfId="122" priority="107" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",J22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="121" priority="102" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="103" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="104" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="118" priority="99" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="100" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="101" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="115" priority="89" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="90" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="113" priority="86" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="87" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="88" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="110" priority="83" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="84" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="85" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="107" priority="73" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="74" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="105" priority="70" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="71" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="72" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="102" priority="67" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="68" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="69" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="99" priority="57" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="58" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="97" priority="54" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="55" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="56" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="94" priority="51" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="52" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="53" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="91" priority="41" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="42" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="89" priority="38" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="39" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="40" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="86" priority="35" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="36" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="37" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="83" priority="33" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="34" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="81" priority="30" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="31" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="32" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="78" priority="27" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="28" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="29" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="75" priority="17" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="18" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="73" priority="14" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="15" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="16" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="70" priority="11" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="12" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="13" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="67" priority="9" operator="containsText" text="MEDIUM">
+  <conditionalFormatting sqref="I21:L22">
+    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="10" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="65" priority="6" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="7" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="63" priority="8" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="60" priority="1" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",I22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="58" priority="3" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -3911,26 +3180,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0768D9F1-4234-49C1-8BF8-F5440FF0513C}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="11" width="21.140625" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="11" width="21.109375" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3950,7 +3219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -3958,10 +3227,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -3970,7 +3239,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3987,15 +3256,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>19</v>
@@ -4004,7 +3273,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -4014,7 +3283,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4024,7 +3293,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
@@ -4053,7 +3322,7 @@
         <v>28</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>30</v>
@@ -4062,9 +3331,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -4078,21 +3347,21 @@
       <c r="K8" s="39"/>
       <c r="L8" s="40"/>
     </row>
-    <row r="9" spans="1:12" ht="160.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="160.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>31</v>
@@ -4108,21 +3377,21 @@
       <c r="K9" s="22"/>
       <c r="L9" s="23"/>
     </row>
-    <row r="10" spans="1:12" ht="173.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="173.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>31</v>
@@ -4138,27 +3407,27 @@
       <c r="K10" s="4"/>
       <c r="L10" s="27"/>
     </row>
-    <row r="11" spans="1:12" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="4" t="s">
@@ -4168,27 +3437,27 @@
       <c r="K11" s="4"/>
       <c r="L11" s="27"/>
     </row>
-    <row r="12" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="4" t="s">
@@ -4198,27 +3467,27 @@
       <c r="K12" s="4"/>
       <c r="L12" s="27"/>
     </row>
-    <row r="13" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="4" t="s">
@@ -4228,27 +3497,27 @@
       <c r="K13" s="4"/>
       <c r="L13" s="27"/>
     </row>
-    <row r="14" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="4" t="s">
@@ -4258,9 +3527,9 @@
       <c r="K14" s="4"/>
       <c r="L14" s="27"/>
     </row>
-    <row r="15" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -4274,18 +3543,18 @@
       <c r="K15" s="39"/>
       <c r="L15" s="40"/>
     </row>
-    <row r="16" spans="1:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="26" t="s">
@@ -4302,22 +3571,22 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="273.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="273.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G17" s="26" t="s">
         <v>31</v>
@@ -4330,18 +3599,18 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="26" t="s">
@@ -4358,18 +3627,18 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="26" t="s">
@@ -4386,18 +3655,18 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="26" t="s">
@@ -4414,18 +3683,18 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="259.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="259.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="26" t="s">
@@ -4442,18 +3711,18 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="275.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="275.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="26" t="s">
@@ -4476,120 +3745,67 @@
     <mergeCell ref="A15:L15"/>
   </mergeCells>
   <conditionalFormatting sqref="B2 I16:L22">
-    <cfRule type="containsText" dxfId="57" priority="56" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="31" priority="56" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="30" priority="57" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I12 I16:I22">
-    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="PASS">
+  <conditionalFormatting sqref="B2">
+    <cfRule type="containsText" dxfId="29" priority="55" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I14 K9:K14">
+    <cfRule type="containsText" dxfId="28" priority="3" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="4" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I14">
+    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="50" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I12 K9:K12">
-    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+  <conditionalFormatting sqref="I16:I22">
+    <cfRule type="containsText" dxfId="23" priority="49" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="50" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20:I21">
+    <cfRule type="containsText" dxfId="21" priority="39" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="40" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:L22">
-    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="19" priority="51" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="49" priority="55" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21:L21">
-    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21:L21">
-    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20:L20">
-    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="MEDIUM">
+  <conditionalFormatting sqref="I20:L21">
+    <cfRule type="containsText" dxfId="18" priority="41" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="42" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="16" priority="43" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="40" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20:L20">
-    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="38" priority="11" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="12" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13 K13">
-    <cfRule type="containsText" dxfId="36" priority="13" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14 K14">
-    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="4" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -4609,26 +3825,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1936D42-EC5B-4A23-B077-0845695AD7C1}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="11" width="21.140625" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="11" width="21.109375" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -4648,7 +3864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -4656,10 +3872,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -4668,7 +3884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -4685,15 +3901,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>19</v>
@@ -4702,7 +3918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -4712,7 +3928,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4722,7 +3938,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
@@ -4751,7 +3967,7 @@
         <v>28</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>30</v>
@@ -4760,9 +3976,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="38" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -4776,18 +3992,18 @@
       <c r="K8" s="39"/>
       <c r="L8" s="40"/>
     </row>
-    <row r="9" spans="1:12" ht="204" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="204" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="21" t="s">
@@ -4804,18 +4020,18 @@
       <c r="K9" s="22"/>
       <c r="L9" s="23"/>
     </row>
-    <row r="10" spans="1:12" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="26" t="s">
@@ -4832,25 +4048,25 @@
       <c r="K10" s="4"/>
       <c r="L10" s="27"/>
     </row>
-    <row r="11" spans="1:12" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="4" t="s">
@@ -4860,25 +4076,25 @@
       <c r="K11" s="4"/>
       <c r="L11" s="27"/>
     </row>
-    <row r="12" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="4" t="s">
@@ -4888,25 +4104,25 @@
       <c r="K12" s="4"/>
       <c r="L12" s="27"/>
     </row>
-    <row r="13" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="4" t="s">
@@ -4916,25 +4132,25 @@
       <c r="K13" s="4"/>
       <c r="L13" s="27"/>
     </row>
-    <row r="14" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B14" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>87</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>90</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="4" t="s">
@@ -4944,9 +4160,9 @@
       <c r="K14" s="4"/>
       <c r="L14" s="27"/>
     </row>
-    <row r="15" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -4960,18 +4176,18 @@
       <c r="K15" s="39"/>
       <c r="L15" s="40"/>
     </row>
-    <row r="16" spans="1:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="26" t="s">
@@ -4988,22 +4204,22 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G17" s="26" t="s">
         <v>31</v>
@@ -5016,18 +4232,18 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="101.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="101.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="26" t="s">
@@ -5044,18 +4260,18 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="B19" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="25" t="s">
         <v>85</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>88</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="26" t="s">
@@ -5072,18 +4288,18 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="26" t="s">
@@ -5100,18 +4316,18 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="26" t="s">
@@ -5128,18 +4344,18 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="26" t="s">
@@ -5162,120 +4378,67 @@
     <mergeCell ref="A15:L15"/>
   </mergeCells>
   <conditionalFormatting sqref="B2 I16:L22">
-    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="15" priority="28" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="14" priority="29" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I12 I16:I22">
-    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="PASS">
+  <conditionalFormatting sqref="B2">
+    <cfRule type="containsText" dxfId="13" priority="27" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I14 K9:K14">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I14">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I12 K9:K12">
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+  <conditionalFormatting sqref="I16:I22">
+    <cfRule type="containsText" dxfId="7" priority="21" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="22" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20:I21">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:L22">
-    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="3" priority="23" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21:L21">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21:L21">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20:L20">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="MEDIUM">
+  <conditionalFormatting sqref="I20:L21">
+    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="14" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="0" priority="15" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20:L20">
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13 K13">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14 K14">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -5292,6 +4455,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf23f84-f8bc-4e67-ab33-02601704301c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006E296302A21A604AB30B08CDD982AED5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a2e24ddf9d3ff53ecfb88a36bb32033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8bf23f84-f8bc-4e67-ab33-02601704301c" xmlns:ns3="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85173b95bb32453a086c351bdaabae72" ns2:_="" ns3:_="">
     <xsd:import namespace="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
@@ -5514,41 +4697,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf23f84-f8bc-4e67-ab33-02601704301c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDBCEFB4-C136-4DFA-9FAE-3B56459231A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C8A6C0-18BD-4AC2-9685-64609DD34696}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
-    <ds:schemaRef ds:uri="becc6418-98a4-4be0-bb44-3ce60d9e2ca3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5571,9 +4723,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C8A6C0-18BD-4AC2-9685-64609DD34696}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDBCEFB4-C136-4DFA-9FAE-3B56459231A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
+    <ds:schemaRef ds:uri="becc6418-98a4-4be0-bb44-3ce60d9e2ca3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated INITIAL DOCS (.docx)/Test Case v1.0.xlsx
</commit_message>
<xml_diff>
--- a/INITIAL DOCS (.docx)/Test Case v1.0.xlsx
+++ b/INITIAL DOCS (.docx)/Test Case v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofIa\Desktop\APC_2023_2024_T1_G04_Team_AV\INITIAL DOCS (.docx)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBAD207-1346-4D30-9A94-C4B02FCBB0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3605D96-4047-4EC8-9AF6-19CB9C0B3322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Authentication" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="141">
   <si>
     <t>TEST DESCRIPTION</t>
   </si>
@@ -138,9 +138,6 @@
     <t>System will notify that email is invalid.</t>
   </si>
   <si>
-    <t>System will notify that phone number is invalid</t>
-  </si>
-  <si>
     <t>BSSVUC01 - BSSVUC06</t>
   </si>
   <si>
@@ -156,23 +153,13 @@
     <t>Execute by: September 20, 2023</t>
   </si>
   <si>
-    <t>BSSVUC01 Resident Login</t>
-  </si>
-  <si>
     <t>User Authentication</t>
   </si>
   <si>
     <t>The system will notify the user that he/she successfully logged in.</t>
   </si>
   <si>
-    <t xml:space="preserve"> BSSVUC02 Resident Registration</t>
-  </si>
-  <si>
     <t>BSSVUC03 Resident Update Personal Info</t>
-  </si>
-  <si>
-    <t>1. Residents must go to the website and click Online Request
-2. Residents input credentials (email and password) and click log-in button</t>
   </si>
   <si>
     <t>Email: jakersonbermudo98@gmail.com
@@ -200,15 +187,6 @@
 8. Click the link to verify account.  </t>
   </si>
   <si>
-    <t>Resident login with invalid email and password</t>
-  </si>
-  <si>
-    <t>Resident login with valid email but invalid password</t>
-  </si>
-  <si>
-    <t>Resident submit registration with an existing email</t>
-  </si>
-  <si>
     <t>1. Residents must go to the website and click Online Request
 2. Residents input credentials (email and password) and click the log-in button.
 3. Residents click My Profile tab.
@@ -216,31 +194,10 @@
 5. Resident clicks submit button.</t>
   </si>
   <si>
-    <t>Resident has an account.</t>
-  </si>
-  <si>
     <t>Residents should reside in Barangay South Signal Village.</t>
   </si>
   <si>
-    <t>Resident submit registration with invalid password</t>
-  </si>
-  <si>
-    <t>Resident submit registration with invalid captcha</t>
-  </si>
-  <si>
     <t>Resident must be logged-in.</t>
-  </si>
-  <si>
-    <t>Resident did not Accept Data Privacy Notice.</t>
-  </si>
-  <si>
-    <t>Resident did not click the verification link.</t>
-  </si>
-  <si>
-    <t>Resident inputs wrong password.</t>
-  </si>
-  <si>
-    <t>Resident did not put the correct password requirements.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Click the side bar and locate My Profile
@@ -249,22 +206,10 @@
 3.1 Click Save  </t>
   </si>
   <si>
-    <t>Resident did put the correct password requirements.</t>
-  </si>
-  <si>
-    <t>Resident inputs correct password.</t>
-  </si>
-  <si>
     <t>User will notify that the email has already an existing account.</t>
   </si>
   <si>
     <t>Resident submit registration with valid input.</t>
-  </si>
-  <si>
-    <t>Resident accepted the Data Privacy Notice.</t>
-  </si>
-  <si>
-    <t>Resident clicked the verification link.</t>
   </si>
   <si>
     <t>BSSVUC01 Resident Create Request</t>
@@ -322,54 +267,9 @@
     <t xml:space="preserve"> BSSVUC02 Resident Track Concern</t>
   </si>
   <si>
-    <t>Resident login with valid email and password but did not the Captcha</t>
-  </si>
-  <si>
-    <t>The system will notify the user that he/she did not complete the captcha.</t>
-  </si>
-  <si>
-    <t>Resident login with valid email and password and check the Captcha.</t>
-  </si>
-  <si>
-    <t>User will notify that the email already has an existing account.</t>
-  </si>
-  <si>
-    <t>System will notify that customer has successfully created an account.</t>
-  </si>
-  <si>
     <t>Resident must be logged in.</t>
   </si>
   <si>
-    <t>System will update the email address.</t>
-  </si>
-  <si>
-    <t>Resident submit update info in change phone number with valid phone number</t>
-  </si>
-  <si>
-    <t>Resident put the correct password requirements.</t>
-  </si>
-  <si>
-    <t>Resident submit update info in email address with valid email address.</t>
-  </si>
-  <si>
-    <t>Resident submit update info in change email with invalid email address.</t>
-  </si>
-  <si>
-    <t>Resident submit update info in change mobile number with invalid mobile number</t>
-  </si>
-  <si>
-    <t>Resident did not click the Save button..</t>
-  </si>
-  <si>
-    <t>Resident clicked the Save button.</t>
-  </si>
-  <si>
-    <t>System will update the password.</t>
-  </si>
-  <si>
-    <t>System will notify that the user followed the password requirements.</t>
-  </si>
-  <si>
     <t>BSSVTC05</t>
   </si>
   <si>
@@ -388,9 +288,6 @@
     <t>BSSVTC10</t>
   </si>
   <si>
-    <t>BSSVTC011</t>
-  </si>
-  <si>
     <t>BSSVTC12</t>
   </si>
   <si>
@@ -400,36 +297,9 @@
     <t>BSSVTC14</t>
   </si>
   <si>
-    <t>BSSVTC15</t>
-  </si>
-  <si>
-    <t>BSSVTC16</t>
-  </si>
-  <si>
-    <t>BSSVTC17</t>
-  </si>
-  <si>
-    <t>BSSVTC18</t>
-  </si>
-  <si>
-    <t>BSSVTC19</t>
-  </si>
-  <si>
-    <t>BSSVTC20</t>
-  </si>
-  <si>
     <t>BSSVTC21</t>
   </si>
   <si>
-    <t>BSSVTC22</t>
-  </si>
-  <si>
-    <t>BSSVTC23</t>
-  </si>
-  <si>
-    <t>BSSVTC24</t>
-  </si>
-  <si>
     <t>UC04 Resident Reset Password</t>
   </si>
   <si>
@@ -452,6 +322,320 @@
   </si>
   <si>
     <t>TC04</t>
+  </si>
+  <si>
+    <t>Online Request</t>
+  </si>
+  <si>
+    <t>Online Request Module</t>
+  </si>
+  <si>
+    <t>Online Concern</t>
+  </si>
+  <si>
+    <t>Online Concern Module</t>
+  </si>
+  <si>
+    <t>BSSVUC01 Resident Register</t>
+  </si>
+  <si>
+    <t>https://asiapacificcollege.sharepoint.com/:f:/s/QUALITYMI201MI203T12023-2024/ErQ-Ye05BZVFpg1PE5_i5m4BQM3C5MKolLq99mA6WKRq4g?e=0LydPm</t>
+  </si>
+  <si>
+    <t>System will notify user that the registration is successful</t>
+  </si>
+  <si>
+    <t>Resident submit registration with complete and valid input.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BSSVUC02 Resident Login</t>
+  </si>
+  <si>
+    <t>Resident submit registration with invalid input.</t>
+  </si>
+  <si>
+    <t>Residents must have an account</t>
+  </si>
+  <si>
+    <t>1.	Residents must go to the website and click Online Services
+2.	Residents input credentials (email and password) and click log-in button</t>
+  </si>
+  <si>
+    <t>Email: mtaspeli@student.apc.edu.ph
+Password: invalid</t>
+  </si>
+  <si>
+    <t>Notifies user Login failed. Email or Password does not match with our record.</t>
+  </si>
+  <si>
+    <t>System will direct to home page</t>
+  </si>
+  <si>
+    <t>1. Residents must go to the website and click Online Services.
+2. Residents input credentials (email and password) and click the log-in button.
+3. Residents click My Profile tab.
+4. Residents click the edit button besides the information wanted to edit and input necessary information required in the form.
+5. Resident clicks submit button.</t>
+  </si>
+  <si>
+    <t>System displays dashboard.</t>
+  </si>
+  <si>
+    <t>Resident submit invalid credentials and checked captcha.</t>
+  </si>
+  <si>
+    <t>Resident submit valid credentials and checked captcha.</t>
+  </si>
+  <si>
+    <t>Resident submit invalid credentials and unchecked captcha.</t>
+  </si>
+  <si>
+    <t>Resident submit valid credentials and unchecked captcha.</t>
+  </si>
+  <si>
+    <t>BSSVTC11</t>
+  </si>
+  <si>
+    <t>Email: Jakersonbbermudo@gmail.com
+Password: User_123</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email: Jakersonbbermudo@gmail.com
+Password: User_123  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF04A800"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>New Email: srvillamin@student.apc.edu.ph
+Password: User_123</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email: Jakersonbbermudo@gmail.com
+Password: User_123  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF04A800"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">New Email: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>invalid@io.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF04A800"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Password: User_123</t>
+    </r>
+  </si>
+  <si>
+    <t>System will notify user to check the captcha</t>
+  </si>
+  <si>
+    <t>System displays ReCAPTCHA Verification Required.</t>
+  </si>
+  <si>
+    <t>Resident submit new valid email address.</t>
+  </si>
+  <si>
+    <t>Resident submit new invalid email address.</t>
+  </si>
+  <si>
+    <t>Resident submit new valid mobile number.</t>
+  </si>
+  <si>
+    <t>Resident submit new invalid mobile number.</t>
+  </si>
+  <si>
+    <t>System notify user that he/she sucessfully updated his/her email address.</t>
+  </si>
+  <si>
+    <t>System displays "You successfully updated your email!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System will notify user that he/she successfully updated his/her mobile number. </t>
+  </si>
+  <si>
+    <t>System displays "You successfully updated your mobile number!"</t>
+  </si>
+  <si>
+    <t>System notify user that he/she failed to updated his/her mobile number.</t>
+  </si>
+  <si>
+    <t>New Mobile Number: 09983537847</t>
+  </si>
+  <si>
+    <t>New Mobile Number: 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Old Password: User_123</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF04A800"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>New Password: User123@</t>
+    </r>
+  </si>
+  <si>
+    <t>System displays "You successfully updated your PASSWORD!"</t>
+  </si>
+  <si>
+    <t>System will notify user that he/she successfully updated his/her new password.</t>
+  </si>
+  <si>
+    <t>System displays " Uppercase and Lowercase
+ Number(0-9)
+ Special Character (!@#$%^&amp;*_-)
+ Atleast 8 characters"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Old Password: User_123</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>New Password: 123456abc</t>
+    </r>
+  </si>
+  <si>
+    <t>Resident input incorrect old password and valid new password.</t>
+  </si>
+  <si>
+    <t>Resident input correct old password and valid new password.</t>
+  </si>
+  <si>
+    <t>Resident input correct old password and invalid new password.</t>
+  </si>
+  <si>
+    <t>Resident input incorrect old password and invalid new password.</t>
+  </si>
+  <si>
+    <t>System displays "CANNOT CHANGE PASSWORD"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Old Password: User123@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>New Password: User_123</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Old Password: User123@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>New Password: 123456abc</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -461,7 +645,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,6 +693,60 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF04A800"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -765,10 +1003,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -873,9 +1112,6 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -888,11 +1124,27 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="89">
     <dxf>
       <font>
         <color theme="1"/>
@@ -1233,6 +1485,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -1265,21 +1524,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1295,49 +1544,29 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1354,6 +1583,26 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -1363,9 +1612,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1386,34 +1638,17 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1498,43 +1733,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1545,19 +1743,39 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1578,37 +1796,34 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1624,53 +1839,39 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1691,37 +1892,17 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1736,8 +1917,113 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFEAEEF3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFEAEEF3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF04A800"/>
+      <color rgb="FF9E00D0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2046,10 +2332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34081978-D0BE-495A-A8D6-1A011FC4BDD5}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2057,7 +2343,7 @@
     <col min="1" max="1" width="33.109375" customWidth="1"/>
     <col min="2" max="2" width="41.109375" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" customWidth="1"/>
+    <col min="4" max="4" width="61" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" customWidth="1"/>
     <col min="6" max="6" width="20.109375" customWidth="1"/>
     <col min="7" max="7" width="19.88671875" customWidth="1"/>
@@ -2095,10 +2381,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -2126,13 +2412,13 @@
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>19</v>
@@ -2190,7 +2476,7 @@
         <v>28</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>30</v>
@@ -2200,41 +2486,41 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="40"/>
+      <c r="A8" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
     </row>
     <row r="9" spans="1:12" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="21"/>
@@ -2249,23 +2535,23 @@
       <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="25" t="s">
+      <c r="B10" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>50</v>
       </c>
+      <c r="E10" s="40" t="s">
+        <v>96</v>
+      </c>
       <c r="F10" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>31</v>
+        <v>97</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>97</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="4" t="s">
@@ -2279,23 +2565,23 @@
       <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>51</v>
+      <c r="B11" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>96</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="4" t="s">
@@ -2305,874 +2591,647 @@
       <c r="K11" s="4"/>
       <c r="L11" s="27"/>
     </row>
-    <row r="12" spans="1:12" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
+    </row>
+    <row r="13" spans="1:12" ht="134.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="27"/>
-    </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="40"/>
+      <c r="B13" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="27"/>
     </row>
     <row r="14" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="25"/>
+        <v>102</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>113</v>
+      </c>
       <c r="F14" s="26" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="J14" s="27"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="L14" s="27"/>
     </row>
     <row r="15" spans="1:12" ht="273.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="25"/>
+        <v>102</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>103</v>
+      </c>
       <c r="F15" s="26" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="H15" s="26"/>
-      <c r="I15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="27"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L15" s="27"/>
+    </row>
+    <row r="16" spans="1:12" ht="250.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="25"/>
+        <v>102</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>113</v>
+      </c>
       <c r="F16" s="26" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="H16" s="26"/>
-      <c r="I16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="27"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="L16" s="27"/>
+    </row>
+    <row r="17" spans="1:12" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
     </row>
     <row r="18" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>60</v>
+        <v>76</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="25"/>
+        <v>106</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="F18" s="26" t="s">
-        <v>31</v>
+        <v>122</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="J18" s="27"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="L18" s="27"/>
     </row>
     <row r="19" spans="1:12" ht="259.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>60</v>
+      <c r="A19" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>53</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="25"/>
+        <v>106</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>115</v>
+      </c>
       <c r="F19" s="26" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="J19" s="27"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" ht="275.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
+      <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="1:12" ht="269.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="23"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="23"/>
+    </row>
+    <row r="21" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" ht="279" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>60</v>
+      <c r="B21" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>53</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="25"/>
+        <v>51</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>128</v>
+      </c>
       <c r="F21" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>31</v>
+        <v>126</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="4"/>
+      <c r="J21" s="27"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="1:12" ht="288.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="25" t="s">
+      <c r="L21" s="27"/>
+    </row>
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="39"/>
+    </row>
+    <row r="23" spans="1:12" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="26" t="s">
+      <c r="E23" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="H23" s="26"/>
+      <c r="I23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="1:12" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="26"/>
-      <c r="I22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="40"/>
-    </row>
-    <row r="24" spans="1:12" ht="246" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="26" t="s">
-        <v>96</v>
-      </c>
       <c r="G24" s="26" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="H24" s="26"/>
       <c r="I24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="27"/>
-    </row>
-    <row r="25" spans="1:12" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+    </row>
+    <row r="25" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>139</v>
+      </c>
       <c r="F25" s="26" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="27"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="27"/>
-    </row>
-    <row r="26" spans="1:12" ht="269.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+    </row>
+    <row r="26" spans="1:12" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="26"/>
+      <c r="I26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="23"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="23"/>
-    </row>
-    <row r="27" spans="1:12" ht="261.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G27" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J27" s="27"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="27"/>
-    </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="40"/>
-    </row>
-    <row r="29" spans="1:12" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="C29" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="26"/>
-      <c r="I29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-    </row>
-    <row r="30" spans="1:12" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-    </row>
-    <row r="31" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-    </row>
-    <row r="32" spans="1:12" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="G32" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-    </row>
-    <row r="33" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H33" s="26"/>
-      <c r="I33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-    </row>
-    <row r="34" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="G34" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="H34" s="26"/>
-      <c r="I34" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-    </row>
-    <row r="35" spans="1:12" ht="264" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="H35" s="26"/>
-      <c r="I35" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" s="27"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="27"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A22:L22"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2 I14:L20">
-    <cfRule type="containsText" dxfId="86" priority="171" operator="containsText" text="LOW">
+  <conditionalFormatting sqref="B2 I14:I16 K14:K16 I20:I21 K20:K21">
+    <cfRule type="containsText" dxfId="88" priority="195" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="196" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="170" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="84" priority="169" operator="containsText" text="HIGH">
+  <conditionalFormatting sqref="B2 I20:I21 K20:K21">
+    <cfRule type="containsText" dxfId="86" priority="194" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I12 I14:I20 I24:I27 I29">
-    <cfRule type="containsText" dxfId="83" priority="159" operator="containsText" text="FAIL">
+  <conditionalFormatting sqref="I9:I11 I14:I16 I23 I20:I21">
+    <cfRule type="containsText" dxfId="85" priority="184" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I12 I24:I27 K9:K12 K24:K27 K35">
-    <cfRule type="containsText" dxfId="82" priority="166" operator="containsText" text="HIGH">
+  <conditionalFormatting sqref="I9:I11 K9:K11">
+    <cfRule type="containsText" dxfId="84" priority="191" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I12 K9:K12 I24:I27 K24:K27 K35">
-    <cfRule type="containsText" dxfId="81" priority="168" operator="containsText" text="LOW">
+  <conditionalFormatting sqref="I9:I11 K9:K11">
+    <cfRule type="containsText" dxfId="83" priority="192" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="193" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="167" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I20 I29 I9:I12 I24:I27">
-    <cfRule type="containsText" dxfId="79" priority="158" operator="containsText" text="PASS">
+  <conditionalFormatting sqref="I14:I16 I23 I9:I11 I20:I21">
+    <cfRule type="containsText" dxfId="81" priority="183" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I19">
-    <cfRule type="containsText" dxfId="78" priority="139" operator="containsText" text="PASS">
+  <conditionalFormatting sqref="I23">
+    <cfRule type="containsText" dxfId="80" priority="127" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="128" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="129" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23:I24">
+    <cfRule type="containsText" dxfId="77" priority="111" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="112" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="75" priority="113" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="containsText" dxfId="74" priority="114" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="115" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:I25">
+    <cfRule type="containsText" dxfId="72" priority="95" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="96" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="97" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="containsText" dxfId="69" priority="98" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="99" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25:I26">
+    <cfRule type="containsText" dxfId="67" priority="79" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="80" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="81" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="containsText" dxfId="64" priority="82" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="83" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="64" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="65" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I16 K14:K16">
+    <cfRule type="containsText" dxfId="54" priority="188" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="containsText" dxfId="53" priority="24" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="25" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="containsText" dxfId="51" priority="23" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="containsText" dxfId="50" priority="18" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="19" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="containsText" dxfId="48" priority="17" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="containsText" dxfId="47" priority="13" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",I18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="containsText" dxfId="46" priority="14" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="containsText" dxfId="45" priority="15" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="16" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="containsText" dxfId="43" priority="12" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="138" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:I22">
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="42" priority="9" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="74" priority="104" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="103" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="102" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I29)))</formula>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="41" priority="10" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="11" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29:I30">
-    <cfRule type="containsText" dxfId="71" priority="87" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="86" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="88" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I29)))</formula>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="containsText" dxfId="39" priority="5" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="68" priority="90" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="89" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I30)))</formula>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="containsText" dxfId="38" priority="6" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30:I31">
-    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="71" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="70" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I30)))</formula>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="containsText" dxfId="37" priority="7" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="8" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="63" priority="73" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="74" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I31)))</formula>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31:I32">
-    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="55" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="56" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I31)))</formula>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="containsText" dxfId="34" priority="1" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32:I33">
-    <cfRule type="containsText" dxfId="56" priority="38" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="39" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="40" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="53" priority="42" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="41" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33:I34">
-    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="30" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="32" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="48" priority="33" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="34" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34:I35">
-    <cfRule type="containsText" dxfId="46" priority="16" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="15" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="14" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="43" priority="12" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="18" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="17" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="13" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="11" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:L20">
-    <cfRule type="containsText" dxfId="38" priority="163" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:L19">
-    <cfRule type="containsText" dxfId="37" priority="140" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="141" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="142" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21:L22">
-    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{629F5E00-D22C-4947-892D-7421C3143FAC}">
       <formula1>$F$2:$F$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K12 I9:I12 I29:I35 K35 K24:K27 I24:I27 I14:L22" xr:uid="{C2C30F8B-DB06-4741-B9A3-A6684606A9B7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K11 I9:I11 I13:I16 K13:K16 I18:I21 K18:K21 I23:I26" xr:uid="{C2C30F8B-DB06-4741-B9A3-A6684606A9B7}">
       <formula1>$G$2:$G$4</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{7B9277B7-5B64-4CEB-94DA-4A692760B864}"/>
+    <hyperlink ref="E13" r:id="rId2" display="mtaspeli@student.apc.edu.ph" xr:uid="{8A7D535B-C43A-47AA-8EF3-74F03CC7B445}"/>
+    <hyperlink ref="E15" r:id="rId3" display="mtaspeli@student.apc.edu.ph" xr:uid="{8907F5FB-E0E4-48EB-B43A-A3D840032482}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3180,8 +3239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0768D9F1-4234-49C1-8BF8-F5440FF0513C}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView zoomScale="61" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3221,16 +3280,16 @@
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -3258,13 +3317,13 @@
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>19</v>
@@ -3322,7 +3381,7 @@
         <v>28</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>30</v>
@@ -3332,36 +3391,36 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="40"/>
+      <c r="A8" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
     </row>
     <row r="9" spans="1:12" ht="160.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>31</v>
@@ -3382,16 +3441,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>31</v>
@@ -3412,22 +3471,22 @@
         <v>5</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="4" t="s">
@@ -3442,22 +3501,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="4" t="s">
@@ -3469,25 +3528,25 @@
     </row>
     <row r="13" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="4" t="s">
@@ -3499,25 +3558,25 @@
     </row>
     <row r="14" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="4" t="s">
@@ -3528,33 +3587,33 @@
       <c r="L14" s="27"/>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="40"/>
+      <c r="A15" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
     </row>
     <row r="16" spans="1:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="26" t="s">
@@ -3573,20 +3632,20 @@
     </row>
     <row r="17" spans="1:12" ht="273.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="26" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="G17" s="26" t="s">
         <v>31</v>
@@ -3601,16 +3660,16 @@
     </row>
     <row r="18" spans="1:12" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="26" t="s">
@@ -3629,16 +3688,16 @@
     </row>
     <row r="19" spans="1:12" ht="260.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="26" t="s">
@@ -3660,13 +3719,13 @@
         <v>32</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="26" t="s">
@@ -3688,13 +3747,13 @@
         <v>33</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="26" t="s">
@@ -3716,13 +3775,13 @@
         <v>34</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="26" t="s">
@@ -3825,8 +3884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1936D42-EC5B-4A23-B077-0845695AD7C1}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3866,16 +3925,16 @@
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -3903,13 +3962,13 @@
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>19</v>
@@ -3967,7 +4026,7 @@
         <v>28</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>30</v>
@@ -3977,33 +4036,33 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="40"/>
+      <c r="A8" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
     </row>
     <row r="9" spans="1:12" ht="204" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="21" t="s">
@@ -4025,13 +4084,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="26" t="s">
@@ -4053,20 +4112,20 @@
         <v>5</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="4" t="s">
@@ -4081,20 +4140,20 @@
         <v>6</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="4" t="s">
@@ -4106,23 +4165,23 @@
     </row>
     <row r="13" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="4" t="s">
@@ -4134,23 +4193,23 @@
     </row>
     <row r="14" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="4" t="s">
@@ -4161,33 +4220,33 @@
       <c r="L14" s="27"/>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="40"/>
+      <c r="A15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
     </row>
     <row r="16" spans="1:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="26" t="s">
@@ -4206,20 +4265,20 @@
     </row>
     <row r="17" spans="1:12" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="26" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="G17" s="26" t="s">
         <v>31</v>
@@ -4234,16 +4293,16 @@
     </row>
     <row r="18" spans="1:12" ht="101.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="26" t="s">
@@ -4262,16 +4321,16 @@
     </row>
     <row r="19" spans="1:12" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="26" t="s">
@@ -4293,13 +4352,13 @@
         <v>32</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="26" t="s">
@@ -4321,13 +4380,13 @@
         <v>34</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="26" t="s">
@@ -4349,13 +4408,13 @@
         <v>35</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="26" t="s">
@@ -4455,26 +4514,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf23f84-f8bc-4e67-ab33-02601704301c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006E296302A21A604AB30B08CDD982AED5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a2e24ddf9d3ff53ecfb88a36bb32033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8bf23f84-f8bc-4e67-ab33-02601704301c" xmlns:ns3="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85173b95bb32453a086c351bdaabae72" ns2:_="" ns3:_="">
     <xsd:import namespace="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
@@ -4697,10 +4736,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf23f84-f8bc-4e67-ab33-02601704301c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C8A6C0-18BD-4AC2-9685-64609DD34696}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDBCEFB4-C136-4DFA-9FAE-3B56459231A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
+    <ds:schemaRef ds:uri="becc6418-98a4-4be0-bb44-3ce60d9e2ca3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4723,20 +4793,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDBCEFB4-C136-4DFA-9FAE-3B56459231A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C8A6C0-18BD-4AC2-9685-64609DD34696}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
-    <ds:schemaRef ds:uri="becc6418-98a4-4be0-bb44-3ce60d9e2ca3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated Test Case v1.0.xlsx
</commit_message>
<xml_diff>
--- a/INITIAL DOCS (.docx)/Test Case v1.0.xlsx
+++ b/INITIAL DOCS (.docx)/Test Case v1.0.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofIa\Desktop\APC_2023_2024_T1_G04_Team_AV\INITIAL DOCS (.docx)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D335FC-9BA5-40DB-BCA3-1BD1DB1B648F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFAB4D2-2790-4D25-B8A9-798D637CE2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Authentication" sheetId="5" r:id="rId1"/>
     <sheet name="Online Request" sheetId="7" r:id="rId2"/>
     <sheet name="Online Concern" sheetId="9" r:id="rId3"/>
+    <sheet name="Payment Option" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="160">
   <si>
     <t>TEST DESCRIPTION</t>
   </si>
@@ -675,6 +676,23 @@
   </si>
   <si>
     <t>BSSVTC07.1 - BSSVTC08.1</t>
+  </si>
+  <si>
+    <t>Payment Option Module</t>
+  </si>
+  <si>
+    <t>Payment Option</t>
+  </si>
+  <si>
+    <t>BSSVUC09 Resident Payment Option</t>
+  </si>
+  <si>
+    <t>BSSVTC09.1</t>
+  </si>
+  <si>
+    <t>1.	Residents must request valid requirements. 
+2.	Residents must go to the Payment page and click process payment.
+3.	Residents choose payment options and pay their requested requirements</t>
   </si>
 </sst>
 </file>
@@ -1183,24 +1201,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="220">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="109">
     <dxf>
       <font>
         <color theme="1"/>
@@ -1260,20 +1261,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -1305,6 +1292,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -1316,18 +1310,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1364,11 +1351,18 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1395,23 +1389,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1460,6 +1437,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -1490,6 +1477,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -1500,9 +1494,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1581,33 +1578,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
@@ -1704,6 +1674,33 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
@@ -1773,33 +1770,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <fgColor auto="1"/>
           <bgColor rgb="FFEAEEF3"/>
         </patternFill>
@@ -1932,23 +1902,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -1971,6 +1924,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -2162,9 +2125,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2210,16 +2176,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.499984740745262"/>
@@ -2302,997 +2258,6 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3614,7 +2579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34081978-D0BE-495A-A8D6-1A011FC4BDD5}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -4316,535 +3281,182 @@
     <mergeCell ref="A22:L22"/>
   </mergeCells>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="219" priority="325" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="108" priority="324" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="107" priority="325" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="326" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="106" priority="326" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="217" priority="324" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="containsText" dxfId="216" priority="314" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="105" priority="313" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="104" priority="314" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I9)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="321" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="322" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="101" priority="323" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I11">
-    <cfRule type="containsText" dxfId="215" priority="321" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="322" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="323" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+  <conditionalFormatting sqref="I13:I16">
+    <cfRule type="containsText" dxfId="100" priority="111" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="112" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="113" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="114" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="115" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I11">
-    <cfRule type="containsText" dxfId="212" priority="313" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
+  <conditionalFormatting sqref="I18:I20">
+    <cfRule type="containsText" dxfId="95" priority="102" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="103" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="104" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="105" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="211" priority="128" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="129" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="130" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="208" priority="126" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="127" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="206" priority="123" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="124" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="125" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="203" priority="121" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="122" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="201" priority="118" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="119" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="120" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="198" priority="116" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="117" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="196" priority="113" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="114" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="115" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="193" priority="111" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="112" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="191" priority="108" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="109" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="110" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="188" priority="106" operator="containsText" text="PASS">
+  <conditionalFormatting sqref="I18:I21">
+    <cfRule type="containsText" dxfId="91" priority="96" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="107" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19:I20">
-    <cfRule type="containsText" dxfId="186" priority="103" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="104" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="105" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19:I20">
-    <cfRule type="containsText" dxfId="183" priority="101" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="102" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="181" priority="97" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="90" priority="97" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I21)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="98" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="99" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="100" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="180" priority="98" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="99" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="100" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I21)))</formula>
+  <conditionalFormatting sqref="I23:I26">
+    <cfRule type="containsText" dxfId="86" priority="76" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="77" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="78" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="79" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="80" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I23)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="177" priority="96" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I21)))</formula>
+  <conditionalFormatting sqref="K9:K11">
+    <cfRule type="containsText" dxfId="81" priority="61" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="62" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="63" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="64" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="65" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="176" priority="93" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="94" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="95" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I23)))</formula>
+  <conditionalFormatting sqref="K13:K16">
+    <cfRule type="containsText" dxfId="76" priority="41" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="75" priority="42" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="43" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="44" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="45" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="173" priority="91" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="92" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I23)))</formula>
+  <conditionalFormatting sqref="K18:K20">
+    <cfRule type="containsText" dxfId="71" priority="27" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="28" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="29" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="30" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="containsText" dxfId="171" priority="88" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="89" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="90" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="containsText" dxfId="168" priority="86" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="87" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="containsText" dxfId="166" priority="83" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="84" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="85" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="containsText" dxfId="163" priority="81" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="82" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="containsText" dxfId="161" priority="78" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="79" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="80" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="containsText" dxfId="158" priority="76" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="77" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="156" priority="73" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="74" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="75" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="153" priority="71" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="72" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="151" priority="68" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="69" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="70" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="148" priority="66" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="67" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="containsText" dxfId="146" priority="63" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="64" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="65" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="containsText" dxfId="143" priority="61" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="62" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="141" priority="58" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="59" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="60" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="138" priority="56" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="57" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="136" priority="53" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="54" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="55" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="133" priority="51" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="52" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="131" priority="48" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="49" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="50" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="128" priority="46" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="47" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="containsText" dxfId="126" priority="43" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="44" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="45" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="containsText" dxfId="123" priority="41" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="42" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="121" priority="38" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="39" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="40" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="118" priority="36" operator="containsText" text="PASS">
+  <conditionalFormatting sqref="K18:K21">
+    <cfRule type="containsText" dxfId="67" priority="21" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="37" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="containsText" dxfId="116" priority="33" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="34" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="35" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="containsText" dxfId="113" priority="31" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="32" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="111" priority="28" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="29" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="30" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="108" priority="26" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="27" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="106" priority="22" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="66" priority="22" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",K21)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="23" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="24" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="25" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K21)))</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="105" priority="23" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="24" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="25" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="containsText" dxfId="102" priority="21" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="containsText" dxfId="101" priority="18" operator="containsText" text="HIGH">
+  <conditionalFormatting sqref="K23:K26">
+    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="3" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",K23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="19" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="59" priority="4" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",K23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="20" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="58" priority="5" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",K23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="containsText" dxfId="98" priority="16" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="17" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
-    <cfRule type="containsText" dxfId="96" priority="13" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="14" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="15" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
-    <cfRule type="containsText" dxfId="93" priority="11" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="12" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="containsText" dxfId="91" priority="8" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="9" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="10" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="containsText" dxfId="88" priority="6" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="7" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
-    <cfRule type="containsText" dxfId="86" priority="3" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="4" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="5" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
-    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -4869,7 +3481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0768D9F1-4234-49C1-8BF8-F5440FF0513C}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="52" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="52" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -5246,234 +3858,78 @@
     <mergeCell ref="A8:L8"/>
     <mergeCell ref="A14:L14"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2 I15:J15 L15">
-    <cfRule type="containsText" dxfId="81" priority="111" operator="containsText" text="MEDIUM">
+  <conditionalFormatting sqref="B2 I15:J15">
+    <cfRule type="containsText" dxfId="57" priority="111" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="112" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="56" priority="112" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2 I15:J15 L15">
-    <cfRule type="containsText" dxfId="79" priority="110" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
+  <conditionalFormatting sqref="I9:I13">
+    <cfRule type="containsText" dxfId="55" priority="31" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="32" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="33" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="34" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="35" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="78" priority="56" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="50" priority="56" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="57" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="49" priority="57" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="containsText" dxfId="76" priority="53" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="54" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+  <conditionalFormatting sqref="I15:J15 B2">
+    <cfRule type="containsText" dxfId="48" priority="110" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="containsText" dxfId="73" priority="51" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="52" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="containsText" dxfId="71" priority="48" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="49" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="50" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="containsText" dxfId="68" priority="46" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="47" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="containsText" dxfId="66" priority="43" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="44" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="containsText" dxfId="63" priority="41" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="42" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="containsText" dxfId="61" priority="38" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="39" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="containsText" dxfId="58" priority="36" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="37" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="56" priority="33" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="34" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="53" priority="31" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="32" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="51" priority="28" operator="containsText" text="HIGH">
+  <conditionalFormatting sqref="K9:K13">
+    <cfRule type="containsText" dxfId="47" priority="6" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="7" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="8" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",K9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="29" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="44" priority="9" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",K9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="43" priority="10" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="48" priority="26" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="27" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="46" priority="23" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="24" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="containsText" dxfId="41" priority="18" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="19" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="20" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="36" priority="13" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="31" priority="8" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",K13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="42" priority="1" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:L15">
+    <cfRule type="containsText" dxfId="40" priority="3" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",K15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -5500,8 +3956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1936D42-EC5B-4A23-B077-0845695AD7C1}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="53" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="62" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5868,92 +4324,79 @@
     <mergeCell ref="A8:L8"/>
     <mergeCell ref="A14:L14"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2 I15:J15 L15">
-    <cfRule type="containsText" dxfId="21" priority="42" operator="containsText" text="MEDIUM">
+  <conditionalFormatting sqref="B2 I15:J15">
+    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="43" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2 I15:J15 L15">
-    <cfRule type="containsText" dxfId="19" priority="41" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I13 K10:K13">
-    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I13 I15">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="34" priority="16" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I13">
+    <cfRule type="containsText" dxfId="33" priority="17" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="18" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="19" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:J15 B2">
+    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",K9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="HIGH">
+  <conditionalFormatting sqref="K9:K13">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="12" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",K9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="26" priority="13" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",K9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="25" priority="14" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",K9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="PASS">
+  <conditionalFormatting sqref="K10:K13">
+    <cfRule type="containsText" dxfId="24" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",K10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11:K13">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:L15">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",K15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -5969,27 +4412,334 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EDEDCAE-B948-4335-8848-93DD5BCACC73}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="11" width="21.109375" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="44"/>
+    </row>
+    <row r="9" spans="1:12" ht="204" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="23"/>
+    </row>
+    <row r="10" spans="1:12" ht="188.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:12" ht="198" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:12" ht="189" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:12" ht="189" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="44"/>
+    </row>
+    <row r="15" spans="1:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" s="26"/>
+      <c r="I15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A14:L14"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B2 I15:J15">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9 I15">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",I9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",I9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:J15 B2">
+    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",K9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:L15">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9 I9 I15:L15" xr:uid="{9024A54D-AC7F-4B07-9A4A-5BA93BF93C8D}">
+      <formula1>$G$2:$G$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{7D37BE6C-0E0D-49C0-A14C-E7B0F9E7941C}">
+      <formula1>$F$2:$F$4</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf23f84-f8bc-4e67-ab33-02601704301c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006E296302A21A604AB30B08CDD982AED5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a2e24ddf9d3ff53ecfb88a36bb32033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8bf23f84-f8bc-4e67-ab33-02601704301c" xmlns:ns3="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85173b95bb32453a086c351bdaabae72" ns2:_="" ns3:_="">
     <xsd:import namespace="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
@@ -6212,10 +4962,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="becc6418-98a4-4be0-bb44-3ce60d9e2ca3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8bf23f84-f8bc-4e67-ab33-02601704301c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C8A6C0-18BD-4AC2-9685-64609DD34696}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDBCEFB4-C136-4DFA-9FAE-3B56459231A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
+    <ds:schemaRef ds:uri="becc6418-98a4-4be0-bb44-3ce60d9e2ca3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6238,20 +5019,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDBCEFB4-C136-4DFA-9FAE-3B56459231A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C8A6C0-18BD-4AC2-9685-64609DD34696}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8bf23f84-f8bc-4e67-ab33-02601704301c"/>
-    <ds:schemaRef ds:uri="becc6418-98a4-4be0-bb44-3ce60d9e2ca3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>